<commit_message>
Ajout du BIGdicktionnaire de données - Partie 3
</commit_message>
<xml_diff>
--- a/DOCS/DDD.xlsx
+++ b/DOCS/DDD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ludo\Documents\Projet-BDD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\projet_bdd_cnam\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121DFB6F-AF3E-49E0-B023-E8DF4E19B0A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0676D0AC-64E1-40ED-AD28-8CB5E81FF954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0B07ED3-212D-4F07-B3C8-4C6F78661E61}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Nom du contact</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>varchar</t>
-  </si>
-  <si>
     <t>Titre de la news</t>
   </si>
   <si>
@@ -90,15 +87,9 @@
     <t>Type de news</t>
   </si>
   <si>
-    <t>Place de l'évenement</t>
-  </si>
-  <si>
     <t>type d'évenement</t>
   </si>
   <si>
-    <t>Etat de la news</t>
-  </si>
-  <si>
     <t>Participant de l'evenement</t>
   </si>
   <si>
@@ -124,6 +115,24 @@
   </si>
   <si>
     <t>Dictionnaire de données</t>
+  </si>
+  <si>
+    <t>Endroit de l'évenement</t>
+  </si>
+  <si>
+    <t>Auteur de la news</t>
+  </si>
+  <si>
+    <t>Participant à un projet</t>
+  </si>
+  <si>
+    <t>Participant à un évenement</t>
+  </si>
+  <si>
+    <t>nombre de personnes à une évenement</t>
+  </si>
+  <si>
+    <t>Varchar</t>
   </si>
 </sst>
 </file>
@@ -171,22 +180,22 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,334 +511,358 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE3643C-D5DF-48FF-A897-C66266E3FD80}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+    </row>
+    <row r="31" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+    </row>
+    <row r="33" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+    </row>
+    <row r="36" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+    </row>
+    <row r="38" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+    </row>
+    <row r="39" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+    </row>
+    <row r="40" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+    </row>
+    <row r="41" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+    </row>
+    <row r="42" spans="1:2" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A42:B42"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A39:B39"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A26:B26"/>
@@ -838,16 +871,7 @@
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A20:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>